<commit_message>
🪴 Flower art for meetup | Strain NFTs!
</commit_message>
<xml_diff>
--- a/season-2/76-computer-vision/coa-data.xlsx
+++ b/season-2/76-computer-vision/coa-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="100">
   <si>
     <t>coa_parsing_algorithm</t>
   </si>
@@ -106,7 +106,7 @@
     <t>producer_license_number</t>
   </si>
   <si>
-    <t>images</t>
+    <t>image_data</t>
   </si>
   <si>
     <t>metrc_lab_id</t>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>CCL18-0001713</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
   <si>
     <t>1A4060300017A85000001289</t>
@@ -963,92 +960,89 @@
       <c r="AE2" t="s">
         <v>81</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>82</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>83</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>84</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>85</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>86</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>87</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AM2" t="s">
         <v>88</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>89</v>
       </c>
-      <c r="AN2" t="s">
+      <c r="AO2" t="s">
         <v>90</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>91</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>92</v>
       </c>
-      <c r="AQ2" t="s">
+      <c r="AR2" t="s">
+        <v>92</v>
+      </c>
+      <c r="AS2" t="s">
         <v>93</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AT2" t="s">
         <v>93</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AU2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BC2" t="s">
         <v>94</v>
       </c>
-      <c r="AT2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>94</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>95</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BE2" t="s">
         <v>96</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BF2" t="s">
         <v>97</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BG2" t="s">
         <v>98</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BH2" t="s">
         <v>99</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>